<commit_message>
actualizamos el hoario del sexto semestre con clase voluntarias y agregamos los respoando de logica en el cuerto semestre más los del quiento semestre
</commit_message>
<xml_diff>
--- a/6_semestre/horario.xlsx
+++ b/6_semestre/horario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intel\Documents\A-U\6_semestre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93833D3D-FE20-4962-9A8B-4941B2421979}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA4152E-49A9-4E11-9C7B-93DC323252AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t>Lunes</t>
   </si>
@@ -100,13 +100,24 @@
   <si>
     <t>Sistema
 operativo</t>
+  </si>
+  <si>
+    <t>Programacion
+avanzada</t>
+  </si>
+  <si>
+    <t>Logica</t>
+  </si>
+  <si>
+    <t>Logica
+Lab</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,8 +125,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,6 +174,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -171,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -203,6 +234,13 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,7 +594,7 @@
     <col min="6" max="6" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -573,7 +611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -589,7 +627,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -605,7 +643,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -614,14 +652,14 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="8" t="s">
-        <v>16</v>
+      <c r="E4" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -632,12 +670,15 @@
         <v>19</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="13"/>
+    </row>
+    <row r="6" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -649,7 +690,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -665,7 +706,7 @@
       </c>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -681,7 +722,7 @@
       </c>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -689,11 +730,17 @@
       <c r="C9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -701,11 +748,17 @@
         <v>18</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -715,7 +768,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -727,6 +780,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
actualizamos horario y agregamos el primer trabajo de computacion numerica
</commit_message>
<xml_diff>
--- a/6_semestre/horario.xlsx
+++ b/6_semestre/horario.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intel\Documents\A-U\6_semestre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA4152E-49A9-4E11-9C7B-93DC323252AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E9F4F9-1C55-4438-9A87-49BB9AFEF236}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>Lunes</t>
   </si>
@@ -100,24 +100,13 @@
   <si>
     <t>Sistema
 operativo</t>
-  </si>
-  <si>
-    <t>Programacion
-avanzada</t>
-  </si>
-  <si>
-    <t>Logica</t>
-  </si>
-  <si>
-    <t>Logica
-Lab</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,8 +122,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,18 +173,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -202,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -222,25 +206,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,7 +569,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,7 +602,7 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="3"/>
@@ -623,15 +610,13 @@
       <c r="E2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="3"/>
@@ -639,124 +624,106 @@
       <c r="E3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="F3" s="13"/>
     </row>
     <row r="4" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="B4" s="11"/>
       <c r="C4" s="2"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="13"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="C6" s="12"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="3"/>
+      <c r="E7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="3"/>
+      <c r="E8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="8" t="s">
+      <c r="D9" s="12"/>
+      <c r="E9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="12" t="s">
-        <v>24</v>
-      </c>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="8" t="s">
+      <c r="D10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="12" t="s">
-        <v>24</v>
-      </c>
+      <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -764,7 +731,9 @@
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="D11" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>

</xml_diff>